<commit_message>
NC: Print CDD PCR
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_PCR.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_PCR.xlsx
@@ -911,9 +911,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -939,12 +936,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,15 +981,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1024,9 +1006,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1093,22 +1072,43 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1430,8 +1430,8 @@
   </sheetPr>
   <dimension ref="A1:AQ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW10" sqref="AW10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="AB34" sqref="AB34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1735,7 +1735,7 @@
       <c r="U7" s="23"/>
       <c r="V7" s="121">
         <f ca="1">NOW()</f>
-        <v>43672.587823958333</v>
+        <v>43672.803038078702</v>
       </c>
       <c r="W7" s="121"/>
       <c r="X7" s="121"/>
@@ -2046,17 +2046,17 @@
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="90" t="s">
+      <c r="AJ12" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="AK12" s="90"/>
-      <c r="AL12" s="117"/>
-      <c r="AM12" s="50"/>
+      <c r="AK12" s="119"/>
+      <c r="AL12" s="120"/>
+      <c r="AM12" s="49"/>
       <c r="AN12" s="39"/>
       <c r="AQ12" s="40"/>
     </row>
     <row r="13" spans="1:43" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
@@ -2091,7 +2091,7 @@
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
-      <c r="AJ13" s="52"/>
+      <c r="AJ13" s="51"/>
       <c r="AK13" s="30"/>
       <c r="AL13" s="30"/>
       <c r="AM13" s="2"/>
@@ -2099,50 +2099,50 @@
       <c r="AQ13" s="40"/>
     </row>
     <row r="14" spans="1:43" ht="3.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="55"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
-      <c r="Y14" s="55"/>
-      <c r="Z14" s="55"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="56"/>
-      <c r="AC14" s="56"/>
-      <c r="AD14" s="56"/>
-      <c r="AE14" s="55"/>
-      <c r="AF14" s="56"/>
-      <c r="AG14" s="56"/>
-      <c r="AH14" s="56"/>
-      <c r="AI14" s="56"/>
-      <c r="AJ14" s="57"/>
-      <c r="AK14" s="55"/>
-      <c r="AL14" s="55"/>
-      <c r="AM14" s="56"/>
-      <c r="AN14" s="58"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="54"/>
+      <c r="Z14" s="54"/>
+      <c r="AA14" s="55"/>
+      <c r="AB14" s="55"/>
+      <c r="AC14" s="55"/>
+      <c r="AD14" s="55"/>
+      <c r="AE14" s="54"/>
+      <c r="AF14" s="55"/>
+      <c r="AG14" s="55"/>
+      <c r="AH14" s="55"/>
+      <c r="AI14" s="55"/>
+      <c r="AJ14" s="56"/>
+      <c r="AK14" s="54"/>
+      <c r="AL14" s="54"/>
+      <c r="AM14" s="55"/>
+      <c r="AN14" s="57"/>
       <c r="AQ14" s="40"/>
     </row>
     <row r="15" spans="1:43" ht="3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
+      <c r="A15" s="58"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -2185,16 +2185,16 @@
       <c r="AQ15" s="40"/>
     </row>
     <row r="16" spans="1:43" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="109"/>
       <c r="D16" s="118"/>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="119"/>
+      <c r="F16" s="117"/>
       <c r="G16" s="30"/>
       <c r="H16" s="2"/>
       <c r="I16" s="30" t="s">
@@ -2203,16 +2203,16 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="62" t="s">
+      <c r="M16" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="63" t="s">
+      <c r="N16" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O16" s="63" t="s">
+      <c r="O16" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="64"/>
+      <c r="P16" s="61"/>
       <c r="Q16" s="30"/>
       <c r="R16" s="30"/>
       <c r="S16" s="30" t="s">
@@ -2223,50 +2223,50 @@
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
       <c r="X16" s="32"/>
-      <c r="Y16" s="65"/>
-      <c r="Z16" s="65"/>
-      <c r="AA16" s="65"/>
-      <c r="AB16" s="65"/>
-      <c r="AC16" s="65"/>
-      <c r="AD16" s="65"/>
-      <c r="AE16" s="65"/>
-      <c r="AF16" s="65"/>
-      <c r="AG16" s="66"/>
-      <c r="AH16" s="66"/>
-      <c r="AI16" s="66"/>
-      <c r="AJ16" s="66"/>
-      <c r="AK16" s="67"/>
-      <c r="AL16" s="67"/>
-      <c r="AM16" s="68"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="62"/>
+      <c r="AA16" s="62"/>
+      <c r="AB16" s="62"/>
+      <c r="AC16" s="62"/>
+      <c r="AD16" s="62"/>
+      <c r="AE16" s="62"/>
+      <c r="AF16" s="62"/>
+      <c r="AG16" s="63"/>
+      <c r="AH16" s="63"/>
+      <c r="AI16" s="63"/>
+      <c r="AJ16" s="63"/>
+      <c r="AK16" s="64"/>
+      <c r="AL16" s="64"/>
+      <c r="AM16" s="65"/>
       <c r="AN16" s="16"/>
       <c r="AQ16" s="40"/>
     </row>
     <row r="17" spans="1:43" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="109"/>
       <c r="D17" s="118"/>
-      <c r="E17" s="69" t="s">
+      <c r="E17" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="F17" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="70" t="s">
+      <c r="G17" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="72"/>
-      <c r="Q17" s="73"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="70"/>
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
       <c r="T17" s="30"/>
@@ -2293,25 +2293,25 @@
       <c r="AQ17" s="40"/>
     </row>
     <row r="18" spans="1:43" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="109"/>
       <c r="D18" s="118"/>
-      <c r="E18" s="74">
+      <c r="E18" s="71">
         <v>1</v>
       </c>
-      <c r="F18" s="75">
+      <c r="F18" s="72">
         <v>4</v>
       </c>
-      <c r="G18" s="75">
+      <c r="G18" s="72">
         <v>0</v>
       </c>
-      <c r="H18" s="75">
+      <c r="H18" s="72">
         <v>1</v>
       </c>
-      <c r="I18" s="76">
+      <c r="I18" s="73">
         <v>7</v>
       </c>
       <c r="J18" s="30"/>
@@ -2378,12 +2378,12 @@
       <c r="AQ18" s="40"/>
     </row>
     <row r="19" spans="1:43" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="115"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110"/>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
@@ -2407,9 +2407,9 @@
       <c r="W19" s="30"/>
       <c r="X19" s="30"/>
       <c r="Y19" s="30"/>
-      <c r="Z19" s="77"/>
-      <c r="AA19" s="77"/>
-      <c r="AB19" s="77"/>
+      <c r="Z19" s="74"/>
+      <c r="AA19" s="74"/>
+      <c r="AB19" s="74"/>
       <c r="AC19" s="48"/>
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
@@ -2434,12 +2434,12 @@
       <c r="E20" s="48"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="78" t="s">
+      <c r="H20" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="120"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
+      <c r="K20" s="112"/>
       <c r="L20" s="48"/>
       <c r="M20" s="48"/>
       <c r="N20" s="48"/>
@@ -2474,49 +2474,49 @@
       <c r="AQ20" s="40"/>
     </row>
     <row r="21" spans="1:43" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="81"/>
+      <c r="B21" s="114"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="75"/>
       <c r="F21" s="30" t="s">
         <v>22</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="82"/>
-      <c r="S21" s="82"/>
-      <c r="T21" s="82"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="82"/>
-      <c r="W21" s="82"/>
-      <c r="X21" s="82"/>
-      <c r="Y21" s="83"/>
-      <c r="Z21" s="82"/>
-      <c r="AA21" s="82"/>
-      <c r="AB21" s="82"/>
-      <c r="AC21" s="82"/>
-      <c r="AD21" s="82"/>
-      <c r="AE21" s="82"/>
-      <c r="AF21" s="82"/>
-      <c r="AG21" s="82"/>
-      <c r="AH21" s="82"/>
-      <c r="AI21" s="82"/>
-      <c r="AJ21" s="82"/>
-      <c r="AK21" s="82"/>
-      <c r="AL21" s="82"/>
-      <c r="AM21" s="82"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="76"/>
+      <c r="Q21" s="76"/>
+      <c r="R21" s="76"/>
+      <c r="S21" s="76"/>
+      <c r="T21" s="76"/>
+      <c r="U21" s="76"/>
+      <c r="V21" s="76"/>
+      <c r="W21" s="76"/>
+      <c r="X21" s="76"/>
+      <c r="Y21" s="77"/>
+      <c r="Z21" s="76"/>
+      <c r="AA21" s="76"/>
+      <c r="AB21" s="76"/>
+      <c r="AC21" s="76"/>
+      <c r="AD21" s="76"/>
+      <c r="AE21" s="76"/>
+      <c r="AF21" s="76"/>
+      <c r="AG21" s="76"/>
+      <c r="AH21" s="76"/>
+      <c r="AI21" s="76"/>
+      <c r="AJ21" s="76"/>
+      <c r="AK21" s="76"/>
+      <c r="AL21" s="76"/>
+      <c r="AM21" s="76"/>
       <c r="AN21" s="16"/>
       <c r="AQ21" s="40"/>
     </row>
@@ -2524,13 +2524,13 @@
       <c r="A22" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="32">
         <v>0</v>
       </c>
-      <c r="F22" s="65">
+      <c r="F22" s="62">
         <v>1</v>
       </c>
       <c r="G22" s="33">
@@ -2572,7 +2572,7 @@
       <c r="AG22" s="48"/>
       <c r="AH22" s="48"/>
       <c r="AI22" s="48"/>
-      <c r="AJ22" s="50"/>
+      <c r="AJ22" s="49"/>
       <c r="AK22" s="48"/>
       <c r="AL22" s="48"/>
       <c r="AM22" s="48"/>
@@ -2583,19 +2583,19 @@
       <c r="A23" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
@@ -2668,50 +2668,50 @@
       <c r="AQ24" s="40"/>
     </row>
     <row r="25" spans="1:43" ht="3.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="R25" s="55"/>
-      <c r="S25" s="55"/>
-      <c r="T25" s="55"/>
-      <c r="U25" s="55"/>
-      <c r="V25" s="55"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="55"/>
-      <c r="Y25" s="55"/>
-      <c r="Z25" s="55"/>
-      <c r="AA25" s="55"/>
-      <c r="AB25" s="55"/>
-      <c r="AC25" s="55"/>
-      <c r="AD25" s="55"/>
-      <c r="AE25" s="55"/>
-      <c r="AF25" s="55"/>
-      <c r="AG25" s="55"/>
-      <c r="AH25" s="55"/>
-      <c r="AI25" s="55"/>
-      <c r="AJ25" s="55"/>
-      <c r="AK25" s="55"/>
-      <c r="AL25" s="55"/>
-      <c r="AM25" s="55"/>
-      <c r="AN25" s="58"/>
+      <c r="A25" s="79"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="54"/>
+      <c r="S25" s="54"/>
+      <c r="T25" s="54"/>
+      <c r="U25" s="54"/>
+      <c r="V25" s="54"/>
+      <c r="W25" s="54"/>
+      <c r="X25" s="54"/>
+      <c r="Y25" s="54"/>
+      <c r="Z25" s="54"/>
+      <c r="AA25" s="54"/>
+      <c r="AB25" s="54"/>
+      <c r="AC25" s="54"/>
+      <c r="AD25" s="54"/>
+      <c r="AE25" s="54"/>
+      <c r="AF25" s="54"/>
+      <c r="AG25" s="54"/>
+      <c r="AH25" s="54"/>
+      <c r="AI25" s="54"/>
+      <c r="AJ25" s="54"/>
+      <c r="AK25" s="54"/>
+      <c r="AL25" s="54"/>
+      <c r="AM25" s="54"/>
+      <c r="AN25" s="57"/>
       <c r="AQ25" s="40"/>
     </row>
     <row r="26" spans="1:43" s="12" customFormat="1" ht="3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="86"/>
+      <c r="A26" s="80"/>
       <c r="B26" s="30"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
@@ -2751,119 +2751,119 @@
       <c r="AL26" s="30"/>
       <c r="AM26" s="30"/>
       <c r="AN26" s="39"/>
-      <c r="AO26" s="73"/>
-      <c r="AP26" s="73"/>
-      <c r="AQ26" s="73"/>
+      <c r="AO26" s="70"/>
+      <c r="AP26" s="70"/>
+      <c r="AQ26" s="70"/>
     </row>
     <row r="27" spans="1:43" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
       <c r="D27" s="118"/>
-      <c r="E27" s="61" t="s">
+      <c r="E27" s="116" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="119"/>
+      <c r="F27" s="117"/>
       <c r="G27" s="30"/>
       <c r="I27" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="M27" s="62" t="s">
+      <c r="M27" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="N27" s="63" t="s">
+      <c r="N27" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="63" t="s">
+      <c r="O27" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="P27" s="87"/>
+      <c r="P27" s="81"/>
       <c r="Q27" s="30"/>
       <c r="R27" s="30"/>
       <c r="S27" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="T27" s="73"/>
-      <c r="U27" s="73"/>
-      <c r="V27" s="73"/>
-      <c r="W27" s="88"/>
+      <c r="T27" s="70"/>
+      <c r="U27" s="70"/>
+      <c r="V27" s="70"/>
+      <c r="W27" s="82"/>
       <c r="X27" s="32">
         <f t="shared" ref="X27:AF27" si="0">X16</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="65">
+      <c r="Y27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z27" s="65">
+      <c r="Z27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA27" s="65">
+      <c r="AA27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB27" s="65">
+      <c r="AB27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC27" s="65">
+      <c r="AC27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD27" s="65">
+      <c r="AD27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE27" s="65">
+      <c r="AE27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF27" s="65">
+      <c r="AF27" s="62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AG27" s="66"/>
-      <c r="AH27" s="66"/>
-      <c r="AI27" s="66"/>
-      <c r="AJ27" s="66"/>
-      <c r="AK27" s="67"/>
-      <c r="AL27" s="67"/>
-      <c r="AM27" s="68"/>
+      <c r="AG27" s="63"/>
+      <c r="AH27" s="63"/>
+      <c r="AI27" s="63"/>
+      <c r="AJ27" s="63"/>
+      <c r="AK27" s="64"/>
+      <c r="AL27" s="64"/>
+      <c r="AM27" s="65"/>
       <c r="AN27" s="16"/>
-      <c r="AO27" s="73"/>
-      <c r="AP27" s="73"/>
-      <c r="AQ27" s="73"/>
+      <c r="AO27" s="70"/>
+      <c r="AP27" s="70"/>
+      <c r="AQ27" s="70"/>
     </row>
     <row r="28" spans="1:43" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
       <c r="D28" s="118"/>
       <c r="E28" s="32">
         <v>9</v>
       </c>
-      <c r="F28" s="65">
+      <c r="F28" s="62">
         <v>0</v>
       </c>
-      <c r="G28" s="65">
+      <c r="G28" s="62">
         <v>0</v>
       </c>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="66"/>
-      <c r="L28" s="66"/>
-      <c r="M28" s="66"/>
-      <c r="N28" s="66"/>
-      <c r="O28" s="66"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="89"/>
-      <c r="R28" s="73"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="83"/>
+      <c r="R28" s="70"/>
       <c r="S28" s="30"/>
       <c r="T28" s="30"/>
       <c r="U28" s="30"/>
@@ -2886,30 +2886,30 @@
       <c r="AL28" s="30"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="16"/>
-      <c r="AO28" s="73"/>
-      <c r="AP28" s="73"/>
-      <c r="AQ28" s="73"/>
+      <c r="AO28" s="70"/>
+      <c r="AP28" s="70"/>
+      <c r="AQ28" s="70"/>
     </row>
     <row r="29" spans="1:43" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
       <c r="D29" s="118"/>
-      <c r="E29" s="74">
+      <c r="E29" s="71">
         <v>0</v>
       </c>
-      <c r="F29" s="75">
+      <c r="F29" s="72">
         <v>0</v>
       </c>
-      <c r="G29" s="75">
+      <c r="G29" s="72">
         <v>2</v>
       </c>
-      <c r="H29" s="75">
+      <c r="H29" s="72">
         <v>0</v>
       </c>
-      <c r="I29" s="76">
+      <c r="I29" s="73">
         <v>4</v>
       </c>
       <c r="J29" s="30"/>
@@ -2972,17 +2972,17 @@
         <v>1</v>
       </c>
       <c r="AN29" s="16"/>
-      <c r="AO29" s="73"/>
-      <c r="AP29" s="73"/>
-      <c r="AQ29" s="73"/>
+      <c r="AO29" s="70"/>
+      <c r="AP29" s="70"/>
+      <c r="AQ29" s="70"/>
     </row>
     <row r="30" spans="1:43" s="12" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="115"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="110"/>
       <c r="E30" s="48"/>
       <c r="F30" s="48"/>
       <c r="G30" s="48"/>
@@ -3005,9 +3005,9 @@
       <c r="W30" s="30"/>
       <c r="X30" s="30"/>
       <c r="Y30" s="30"/>
-      <c r="Z30" s="77"/>
-      <c r="AA30" s="77"/>
-      <c r="AB30" s="77"/>
+      <c r="Z30" s="74"/>
+      <c r="AA30" s="74"/>
+      <c r="AB30" s="74"/>
       <c r="AC30" s="48"/>
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
@@ -3020,9 +3020,9 @@
       <c r="AL30" s="30"/>
       <c r="AM30" s="30"/>
       <c r="AN30" s="16"/>
-      <c r="AO30" s="73"/>
-      <c r="AP30" s="73"/>
-      <c r="AQ30" s="73"/>
+      <c r="AO30" s="70"/>
+      <c r="AP30" s="70"/>
+      <c r="AQ30" s="70"/>
     </row>
     <row r="31" spans="1:43" s="12" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47" t="s">
@@ -3032,13 +3032,13 @@
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
       <c r="E31" s="48"/>
-      <c r="H31" s="90" t="s">
+      <c r="H31" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="90"/>
-      <c r="J31" s="90"/>
-      <c r="K31" s="117"/>
-      <c r="L31" s="91"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="120"/>
+      <c r="L31" s="84"/>
       <c r="M31" s="48"/>
       <c r="N31" s="48"/>
       <c r="O31" s="48"/>
@@ -3062,18 +3062,18 @@
       <c r="AL31" s="48"/>
       <c r="AM31" s="48"/>
       <c r="AN31" s="16"/>
-      <c r="AO31" s="73"/>
-      <c r="AP31" s="73"/>
-      <c r="AQ31" s="73"/>
+      <c r="AO31" s="70"/>
+      <c r="AP31" s="70"/>
+      <c r="AQ31" s="70"/>
     </row>
     <row r="32" spans="1:43" s="12" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="116"/>
-      <c r="E32" s="81"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="75"/>
       <c r="F32" s="30" t="s">
         <v>22</v>
       </c>
@@ -3110,19 +3110,19 @@
       <c r="AL32" s="48"/>
       <c r="AM32" s="48"/>
       <c r="AN32" s="16"/>
-      <c r="AQ32" s="73"/>
+      <c r="AQ32" s="70"/>
     </row>
     <row r="33" spans="1:43" s="12" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="84"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
       <c r="E33" s="32">
         <v>0</v>
       </c>
-      <c r="F33" s="65">
+      <c r="F33" s="62">
         <v>1</v>
       </c>
       <c r="G33" s="33">
@@ -3161,32 +3161,32 @@
       <c r="AG33" s="48"/>
       <c r="AH33" s="48"/>
       <c r="AI33" s="48"/>
-      <c r="AJ33" s="50"/>
+      <c r="AJ33" s="49"/>
       <c r="AK33" s="48"/>
       <c r="AL33" s="48"/>
       <c r="AM33" s="48"/>
       <c r="AN33" s="39"/>
-      <c r="AO33" s="73"/>
-      <c r="AP33" s="73"/>
-      <c r="AQ33" s="73"/>
+      <c r="AO33" s="70"/>
+      <c r="AP33" s="70"/>
+      <c r="AQ33" s="70"/>
     </row>
     <row r="34" spans="1:43" s="12" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="60" t="s">
+      <c r="A34" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
@@ -3213,79 +3213,79 @@
       <c r="AL34" s="30"/>
       <c r="AM34" s="30"/>
       <c r="AN34" s="39"/>
-      <c r="AO34" s="73"/>
-      <c r="AP34" s="73"/>
-      <c r="AQ34" s="73"/>
+      <c r="AO34" s="70"/>
+      <c r="AP34" s="70"/>
+      <c r="AQ34" s="70"/>
     </row>
     <row r="35" spans="1:43" s="12" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="93"/>
-      <c r="N35" s="93"/>
-      <c r="O35" s="93"/>
-      <c r="P35" s="93"/>
-      <c r="Q35" s="93"/>
-      <c r="R35" s="93"/>
-      <c r="S35" s="93"/>
-      <c r="T35" s="93"/>
-      <c r="U35" s="93"/>
-      <c r="V35" s="93"/>
-      <c r="W35" s="93"/>
-      <c r="X35" s="93"/>
-      <c r="Y35" s="93"/>
-      <c r="Z35" s="93"/>
-      <c r="AA35" s="93"/>
-      <c r="AB35" s="93"/>
-      <c r="AC35" s="93"/>
-      <c r="AD35" s="93"/>
-      <c r="AE35" s="93"/>
-      <c r="AF35" s="93"/>
-      <c r="AG35" s="93"/>
-      <c r="AH35" s="93"/>
-      <c r="AI35" s="93"/>
-      <c r="AJ35" s="93"/>
-      <c r="AK35" s="93"/>
-      <c r="AL35" s="93"/>
-      <c r="AM35" s="93"/>
-      <c r="AN35" s="94"/>
-      <c r="AO35" s="73"/>
-      <c r="AP35" s="73"/>
-      <c r="AQ35" s="73"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="86"/>
+      <c r="D35" s="86"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="86"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="86"/>
+      <c r="J35" s="86"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="86"/>
+      <c r="M35" s="86"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="86"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="86"/>
+      <c r="R35" s="86"/>
+      <c r="S35" s="86"/>
+      <c r="T35" s="86"/>
+      <c r="U35" s="86"/>
+      <c r="V35" s="86"/>
+      <c r="W35" s="86"/>
+      <c r="X35" s="86"/>
+      <c r="Y35" s="86"/>
+      <c r="Z35" s="86"/>
+      <c r="AA35" s="86"/>
+      <c r="AB35" s="86"/>
+      <c r="AC35" s="86"/>
+      <c r="AD35" s="86"/>
+      <c r="AE35" s="86"/>
+      <c r="AF35" s="86"/>
+      <c r="AG35" s="86"/>
+      <c r="AH35" s="86"/>
+      <c r="AI35" s="86"/>
+      <c r="AJ35" s="86"/>
+      <c r="AK35" s="86"/>
+      <c r="AL35" s="86"/>
+      <c r="AM35" s="86"/>
+      <c r="AN35" s="87"/>
+      <c r="AO35" s="70"/>
+      <c r="AP35" s="70"/>
+      <c r="AQ35" s="70"/>
     </row>
     <row r="36" spans="1:43" s="12" customFormat="1" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="89"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="73"/>
-      <c r="T36" s="73"/>
-      <c r="U36" s="73"/>
-      <c r="AN36" s="95"/>
-      <c r="AQ36" s="73"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="70"/>
+      <c r="M36" s="70"/>
+      <c r="N36" s="70"/>
+      <c r="O36" s="70"/>
+      <c r="P36" s="70"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="70"/>
+      <c r="S36" s="70"/>
+      <c r="T36" s="70"/>
+      <c r="U36" s="70"/>
+      <c r="AN36" s="88"/>
+      <c r="AQ36" s="70"/>
     </row>
     <row r="37" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="47"/>
@@ -3303,38 +3303,38 @@
       <c r="M37" s="30"/>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
-      <c r="P37" s="96" t="s">
+      <c r="P37" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="Q37" s="97"/>
-      <c r="R37" s="97"/>
-      <c r="S37" s="97"/>
-      <c r="T37" s="97"/>
-      <c r="U37" s="98"/>
-      <c r="V37" s="98"/>
-      <c r="W37" s="98"/>
-      <c r="X37" s="99"/>
-      <c r="Y37" s="97" t="s">
+      <c r="Q37" s="90"/>
+      <c r="R37" s="90"/>
+      <c r="S37" s="90"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="91"/>
+      <c r="V37" s="91"/>
+      <c r="W37" s="91"/>
+      <c r="X37" s="92"/>
+      <c r="Y37" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="Z37" s="97"/>
-      <c r="AA37" s="98"/>
-      <c r="AB37" s="97"/>
-      <c r="AC37" s="99"/>
-      <c r="AD37" s="97" t="s">
+      <c r="Z37" s="90"/>
+      <c r="AA37" s="91"/>
+      <c r="AB37" s="90"/>
+      <c r="AC37" s="92"/>
+      <c r="AD37" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AE37" s="97"/>
-      <c r="AF37" s="98"/>
-      <c r="AG37" s="97"/>
-      <c r="AH37" s="99"/>
-      <c r="AI37" s="96" t="s">
+      <c r="AE37" s="90"/>
+      <c r="AF37" s="91"/>
+      <c r="AG37" s="90"/>
+      <c r="AH37" s="92"/>
+      <c r="AI37" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="AJ37" s="97"/>
-      <c r="AK37" s="97"/>
-      <c r="AL37" s="97"/>
-      <c r="AM37" s="99"/>
+      <c r="AJ37" s="90"/>
+      <c r="AK37" s="90"/>
+      <c r="AL37" s="90"/>
+      <c r="AM37" s="92"/>
       <c r="AN37" s="16"/>
     </row>
     <row r="38" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3353,30 +3353,30 @@
       <c r="M38" s="30"/>
       <c r="N38" s="30"/>
       <c r="O38" s="30"/>
-      <c r="P38" s="100"/>
-      <c r="Q38" s="101"/>
-      <c r="R38" s="101"/>
-      <c r="S38" s="101"/>
-      <c r="T38" s="101"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="94"/>
+      <c r="T38" s="94"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
       <c r="W38" s="2"/>
-      <c r="X38" s="102"/>
-      <c r="Y38" s="103"/>
-      <c r="Z38" s="104"/>
-      <c r="AA38" s="104"/>
-      <c r="AB38" s="104"/>
-      <c r="AC38" s="105"/>
-      <c r="AD38" s="103"/>
-      <c r="AE38" s="104"/>
-      <c r="AF38" s="104"/>
-      <c r="AG38" s="104"/>
-      <c r="AH38" s="105"/>
-      <c r="AI38" s="103"/>
-      <c r="AJ38" s="104"/>
-      <c r="AK38" s="104"/>
-      <c r="AL38" s="104"/>
-      <c r="AM38" s="105"/>
+      <c r="X38" s="95"/>
+      <c r="Y38" s="96"/>
+      <c r="Z38" s="97"/>
+      <c r="AA38" s="97"/>
+      <c r="AB38" s="97"/>
+      <c r="AC38" s="98"/>
+      <c r="AD38" s="96"/>
+      <c r="AE38" s="97"/>
+      <c r="AF38" s="97"/>
+      <c r="AG38" s="97"/>
+      <c r="AH38" s="98"/>
+      <c r="AI38" s="96"/>
+      <c r="AJ38" s="97"/>
+      <c r="AK38" s="97"/>
+      <c r="AL38" s="97"/>
+      <c r="AM38" s="98"/>
       <c r="AN38" s="16"/>
     </row>
     <row r="39" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3395,73 +3395,73 @@
       <c r="M39" s="30"/>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
-      <c r="P39" s="100"/>
-      <c r="Q39" s="101"/>
-      <c r="R39" s="101"/>
-      <c r="S39" s="101"/>
-      <c r="T39" s="101"/>
+      <c r="P39" s="93"/>
+      <c r="Q39" s="94"/>
+      <c r="R39" s="94"/>
+      <c r="S39" s="94"/>
+      <c r="T39" s="94"/>
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="102"/>
-      <c r="Y39" s="103"/>
-      <c r="Z39" s="104"/>
-      <c r="AA39" s="104"/>
-      <c r="AB39" s="104"/>
-      <c r="AC39" s="105"/>
-      <c r="AD39" s="103"/>
-      <c r="AE39" s="104"/>
-      <c r="AF39" s="104"/>
-      <c r="AG39" s="104"/>
-      <c r="AH39" s="105"/>
-      <c r="AI39" s="103"/>
-      <c r="AJ39" s="104"/>
-      <c r="AK39" s="104"/>
-      <c r="AL39" s="104"/>
-      <c r="AM39" s="105"/>
+      <c r="X39" s="95"/>
+      <c r="Y39" s="96"/>
+      <c r="Z39" s="97"/>
+      <c r="AA39" s="97"/>
+      <c r="AB39" s="97"/>
+      <c r="AC39" s="98"/>
+      <c r="AD39" s="96"/>
+      <c r="AE39" s="97"/>
+      <c r="AF39" s="97"/>
+      <c r="AG39" s="97"/>
+      <c r="AH39" s="98"/>
+      <c r="AI39" s="96"/>
+      <c r="AJ39" s="97"/>
+      <c r="AK39" s="97"/>
+      <c r="AL39" s="97"/>
+      <c r="AM39" s="98"/>
       <c r="AN39" s="16"/>
     </row>
     <row r="40" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106"/>
-      <c r="B40" s="107"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="107"/>
-      <c r="F40" s="107"/>
-      <c r="G40" s="107"/>
-      <c r="H40" s="107"/>
-      <c r="I40" s="107"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="107"/>
-      <c r="N40" s="107"/>
-      <c r="O40" s="107"/>
-      <c r="P40" s="108"/>
-      <c r="Q40" s="109"/>
-      <c r="R40" s="109"/>
-      <c r="S40" s="109"/>
-      <c r="T40" s="109"/>
-      <c r="U40" s="107"/>
-      <c r="V40" s="107"/>
-      <c r="W40" s="107"/>
-      <c r="X40" s="110"/>
-      <c r="Y40" s="111"/>
-      <c r="Z40" s="112"/>
-      <c r="AA40" s="112"/>
-      <c r="AB40" s="112"/>
-      <c r="AC40" s="113"/>
-      <c r="AD40" s="111"/>
-      <c r="AE40" s="112"/>
-      <c r="AF40" s="112"/>
-      <c r="AG40" s="112"/>
-      <c r="AH40" s="113"/>
-      <c r="AI40" s="111"/>
-      <c r="AJ40" s="112"/>
-      <c r="AK40" s="112"/>
-      <c r="AL40" s="112"/>
-      <c r="AM40" s="113"/>
-      <c r="AN40" s="114"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="100"/>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="100"/>
+      <c r="J40" s="100"/>
+      <c r="K40" s="100"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="100"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="101"/>
+      <c r="Q40" s="102"/>
+      <c r="R40" s="102"/>
+      <c r="S40" s="102"/>
+      <c r="T40" s="102"/>
+      <c r="U40" s="100"/>
+      <c r="V40" s="100"/>
+      <c r="W40" s="100"/>
+      <c r="X40" s="103"/>
+      <c r="Y40" s="104"/>
+      <c r="Z40" s="105"/>
+      <c r="AA40" s="105"/>
+      <c r="AB40" s="105"/>
+      <c r="AC40" s="106"/>
+      <c r="AD40" s="104"/>
+      <c r="AE40" s="105"/>
+      <c r="AF40" s="105"/>
+      <c r="AG40" s="105"/>
+      <c r="AH40" s="106"/>
+      <c r="AI40" s="104"/>
+      <c r="AJ40" s="105"/>
+      <c r="AK40" s="105"/>
+      <c r="AL40" s="105"/>
+      <c r="AM40" s="106"/>
+      <c r="AN40" s="107"/>
     </row>
     <row r="41" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A41" s="40"/>
@@ -3490,6 +3490,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="V7:AD7"/>
+    <mergeCell ref="AJ12:AL12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="A21:D21"/>
@@ -3500,13 +3507,6 @@
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="V7:AD7"/>
-    <mergeCell ref="AJ12:AL12"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Entry: Updated NC, XML Accs & Optimized DM: Accs
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_PCR.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_PCR.xlsx
@@ -1078,9 +1078,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1095,24 +1113,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1431,7 +1431,7 @@
   <dimension ref="A1:AQ41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="AB34" sqref="AB34"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1733,18 +1733,18 @@
       </c>
       <c r="T7" s="22"/>
       <c r="U7" s="23"/>
-      <c r="V7" s="121">
+      <c r="V7" s="112">
         <f ca="1">NOW()</f>
-        <v>43672.803038078702</v>
-      </c>
-      <c r="W7" s="121"/>
-      <c r="X7" s="121"/>
-      <c r="Y7" s="121"/>
-      <c r="Z7" s="121"/>
-      <c r="AA7" s="121"/>
-      <c r="AB7" s="121"/>
-      <c r="AC7" s="121"/>
-      <c r="AD7" s="121"/>
+        <v>43675.451223263888</v>
+      </c>
+      <c r="W7" s="112"/>
+      <c r="X7" s="112"/>
+      <c r="Y7" s="112"/>
+      <c r="Z7" s="112"/>
+      <c r="AA7" s="112"/>
+      <c r="AB7" s="112"/>
+      <c r="AC7" s="112"/>
+      <c r="AD7" s="112"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="24"/>
       <c r="AG7" s="25"/>
@@ -2046,11 +2046,11 @@
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
-      <c r="AJ12" s="119" t="s">
+      <c r="AJ12" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="AK12" s="119"/>
-      <c r="AL12" s="120"/>
+      <c r="AK12" s="113"/>
+      <c r="AL12" s="114"/>
       <c r="AM12" s="49"/>
       <c r="AN12" s="39"/>
       <c r="AQ12" s="40"/>
@@ -2190,11 +2190,11 @@
       </c>
       <c r="B16" s="109"/>
       <c r="C16" s="109"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="116" t="s">
+      <c r="D16" s="110"/>
+      <c r="E16" s="115" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="117"/>
+      <c r="F16" s="116"/>
       <c r="G16" s="30"/>
       <c r="H16" s="2"/>
       <c r="I16" s="30" t="s">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B17" s="109"/>
       <c r="C17" s="109"/>
-      <c r="D17" s="118"/>
+      <c r="D17" s="110"/>
       <c r="E17" s="66" t="s">
         <v>51</v>
       </c>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="B18" s="109"/>
       <c r="C18" s="109"/>
-      <c r="D18" s="118"/>
+      <c r="D18" s="110"/>
       <c r="E18" s="71">
         <v>1</v>
       </c>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="B19" s="109"/>
       <c r="C19" s="109"/>
-      <c r="D19" s="110"/>
+      <c r="D19" s="111"/>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
@@ -2434,12 +2434,12 @@
       <c r="E20" s="48"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="111" t="s">
+      <c r="H20" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
-      <c r="K20" s="112"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="117"/>
+      <c r="K20" s="118"/>
       <c r="L20" s="48"/>
       <c r="M20" s="48"/>
       <c r="N20" s="48"/>
@@ -2474,12 +2474,12 @@
       <c r="AQ20" s="40"/>
     </row>
     <row r="21" spans="1:43" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="113" t="s">
+      <c r="A21" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
-      <c r="D21" s="115"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="121"/>
       <c r="E21" s="75"/>
       <c r="F21" s="30" t="s">
         <v>22</v>
@@ -2761,11 +2761,11 @@
       </c>
       <c r="B27" s="109"/>
       <c r="C27" s="109"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="116" t="s">
+      <c r="D27" s="110"/>
+      <c r="E27" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="117"/>
+      <c r="F27" s="116"/>
       <c r="G27" s="30"/>
       <c r="I27" s="30" t="s">
         <v>11</v>
@@ -2789,42 +2789,15 @@
       <c r="U27" s="70"/>
       <c r="V27" s="70"/>
       <c r="W27" s="82"/>
-      <c r="X27" s="32">
-        <f t="shared" ref="X27:AF27" si="0">X16</f>
-        <v>0</v>
-      </c>
-      <c r="Y27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF27" s="62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="62"/>
+      <c r="AA27" s="62"/>
+      <c r="AB27" s="62"/>
+      <c r="AC27" s="62"/>
+      <c r="AD27" s="62"/>
+      <c r="AE27" s="62"/>
+      <c r="AF27" s="62"/>
       <c r="AG27" s="63"/>
       <c r="AH27" s="63"/>
       <c r="AI27" s="63"/>
@@ -2843,7 +2816,7 @@
       </c>
       <c r="B28" s="109"/>
       <c r="C28" s="109"/>
-      <c r="D28" s="118"/>
+      <c r="D28" s="110"/>
       <c r="E28" s="32">
         <v>9</v>
       </c>
@@ -2896,7 +2869,7 @@
       </c>
       <c r="B29" s="109"/>
       <c r="C29" s="109"/>
-      <c r="D29" s="118"/>
+      <c r="D29" s="110"/>
       <c r="E29" s="71">
         <v>0</v>
       </c>
@@ -2982,7 +2955,7 @@
       </c>
       <c r="B30" s="109"/>
       <c r="C30" s="109"/>
-      <c r="D30" s="110"/>
+      <c r="D30" s="111"/>
       <c r="E30" s="48"/>
       <c r="F30" s="48"/>
       <c r="G30" s="48"/>
@@ -3032,12 +3005,12 @@
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
       <c r="E31" s="48"/>
-      <c r="H31" s="119" t="s">
+      <c r="H31" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="119"/>
-      <c r="J31" s="119"/>
-      <c r="K31" s="120"/>
+      <c r="I31" s="113"/>
+      <c r="J31" s="113"/>
+      <c r="K31" s="114"/>
       <c r="L31" s="84"/>
       <c r="M31" s="48"/>
       <c r="N31" s="48"/>
@@ -3067,12 +3040,12 @@
       <c r="AQ31" s="70"/>
     </row>
     <row r="32" spans="1:43" s="12" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="113" t="s">
+      <c r="A32" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="114"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
+      <c r="B32" s="120"/>
+      <c r="C32" s="120"/>
+      <c r="D32" s="121"/>
       <c r="E32" s="75"/>
       <c r="F32" s="30" t="s">
         <v>22</v>
@@ -3176,7 +3149,7 @@
       </c>
       <c r="B34" s="109"/>
       <c r="C34" s="109"/>
-      <c r="D34" s="110"/>
+      <c r="D34" s="111"/>
       <c r="E34" s="49"/>
       <c r="F34" s="49"/>
       <c r="G34" s="49"/>
@@ -3490,13 +3463,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="V7:AD7"/>
-    <mergeCell ref="AJ12:AL12"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="A21:D21"/>
@@ -3507,6 +3473,13 @@
     <mergeCell ref="A28:D28"/>
     <mergeCell ref="A30:D30"/>
     <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="V7:AD7"/>
+    <mergeCell ref="AJ12:AL12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>

</xml_diff>